<commit_message>
Refactor .gitignore to include file exclusion patterns
</commit_message>
<xml_diff>
--- a/test_data_masterplan.xlsx
+++ b/test_data_masterplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_golang\cmd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_fastapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3E7702-06F5-48F2-91FA-F628D63EB89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993C0887-230B-4411-B3E6-7FCCBC5C8FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1328,7 +1328,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2">
-        <v>44880</v>
+        <v>45545</v>
       </c>
       <c r="B3" s="2">
         <v>44930</v>

</xml_diff>

<commit_message>
Refactor generate_masterplan.py to improve error handling and data validation
</commit_message>
<xml_diff>
--- a/test_data_masterplan.xlsx
+++ b/test_data_masterplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\visual_mandiri_informatika\surgery\backend_surgery_fastapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993C0887-230B-4411-B3E6-7FCCBC5C8FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0D5A73-8839-49BE-A039-B82BEACD084B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1328,7 +1328,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>

</xml_diff>